<commit_message>
Shorted environment names for integration test cases
</commit_message>
<xml_diff>
--- a/input_data/2003/basic_posting_flows.milestones/for_mls.big-rocks.journeys.a6i.xlsx
+++ b/input_data/2003/basic_posting_flows.milestones/for_mls.big-rocks.journeys.a6i.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\test_db\input_data\2003\basic_posting_flows.milestones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7672094D-D593-4D32-B23B-9E82F6EE622D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571D9736-AF70-4EE8-89E9-CA51C5E6AA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
     <t>D2:G48</t>
   </si>
   <si>
-    <t>JackHenry</t>
+    <t>Alias de Enrique</t>
   </si>
 </sst>
 </file>
@@ -726,7 +726,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>